<commit_message>
id 9 backlog - essencial
</commit_message>
<xml_diff>
--- a/Documentação/Backlog.xlsx
+++ b/Documentação/Backlog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\camil\Desktop\Github\Pyxis\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\Pyxis\Pyxis\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B0D415-EF51-44C7-B24F-5CFF72B7672D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689AE715-7AAD-4ECF-91CB-B2D42472B4CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DDB84036-6717-47E7-8D2B-220647BD24A7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DDB84036-6717-47E7-8D2B-220647BD24A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -155,7 +155,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -178,14 +178,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,20 +514,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762B3419-BE5B-45F0-ACDC-E0F8E076A4B4}">
   <dimension ref="A3:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.6640625" customWidth="1"/>
-    <col min="4" max="4" width="88.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.5546875" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" customWidth="1"/>
+    <col min="4" max="4" width="88.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -535,7 +547,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -551,7 +563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -567,7 +579,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>3</v>
       </c>
@@ -583,7 +595,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>4</v>
       </c>
@@ -599,7 +611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>5</v>
       </c>
@@ -615,7 +627,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>6</v>
       </c>
@@ -631,7 +643,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>7</v>
       </c>
@@ -647,7 +659,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>8</v>
       </c>
@@ -663,7 +675,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>9</v>
       </c>
@@ -672,14 +684,14 @@
         <v>14</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F12" s="2"/>
       <c r="G12" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>10</v>
       </c>
@@ -695,7 +707,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>11</v>
       </c>
@@ -711,7 +723,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>12</v>
       </c>
@@ -727,7 +739,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>13</v>
       </c>
@@ -743,7 +755,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>14</v>
       </c>
@@ -759,7 +771,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>15</v>
       </c>
@@ -775,7 +787,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>16</v>
       </c>
@@ -791,7 +803,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>17</v>
       </c>
@@ -807,7 +819,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>18</v>
       </c>
@@ -823,7 +835,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>19</v>
       </c>
@@ -838,8 +850,9 @@
       <c r="G22" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.3">
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>20</v>
       </c>
@@ -855,7 +868,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -863,7 +876,7 @@
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -871,7 +884,7 @@
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -879,7 +892,7 @@
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -887,7 +900,7 @@
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -895,7 +908,7 @@
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -903,7 +916,7 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -911,7 +924,7 @@
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -919,7 +932,7 @@
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -927,7 +940,7 @@
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
@@ -935,7 +948,7 @@
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -945,7 +958,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -955,7 +968,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -965,7 +978,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -975,7 +988,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -985,7 +998,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -995,7 +1008,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1005,7 +1018,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1015,7 +1028,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1025,7 +1038,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1035,7 +1048,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1045,7 +1058,7 @@
       <c r="G44" s="1"/>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1055,7 +1068,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1065,7 +1078,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1075,7 +1088,7 @@
       <c r="G47" s="1"/>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1086,7 +1099,7 @@
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1097,7 +1110,7 @@
       <c r="H49" s="1"/>
       <c r="I49" s="1"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1108,7 +1121,7 @@
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1119,7 +1132,7 @@
       <c r="H51" s="1"/>
       <c r="I51" s="1"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1130,7 +1143,7 @@
       <c r="H52" s="1"/>
       <c r="I52" s="1"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1141,7 +1154,7 @@
       <c r="H53" s="1"/>
       <c r="I53" s="1"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1152,7 +1165,7 @@
       <c r="H54" s="1"/>
       <c r="I54" s="1"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1163,7 +1176,7 @@
       <c r="H55" s="1"/>
       <c r="I55" s="1"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1174,7 +1187,7 @@
       <c r="H56" s="1"/>
       <c r="I56" s="1"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1185,7 +1198,7 @@
       <c r="H57" s="1"/>
       <c r="I57" s="1"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1196,7 +1209,7 @@
       <c r="H58" s="1"/>
       <c r="I58" s="1"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1207,7 +1220,7 @@
       <c r="H59" s="1"/>
       <c r="I59" s="1"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1218,7 +1231,7 @@
       <c r="H60" s="1"/>
       <c r="I60" s="1"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1229,7 +1242,7 @@
       <c r="H61" s="1"/>
       <c r="I61" s="1"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>

</xml_diff>

<commit_message>
backlog e backlog ppt
</commit_message>
<xml_diff>
--- a/Documentação/Backlog.xlsx
+++ b/Documentação/Backlog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Guilherme\Desktop\Pyxis\Pyxis\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689AE715-7AAD-4ECF-91CB-B2D42472B4CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55FD86D-95ED-498F-AA21-FB260C1D9E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DDB84036-6717-47E7-8D2B-220647BD24A7}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="34">
   <si>
     <t>ID</t>
   </si>
@@ -126,13 +126,22 @@
   </si>
   <si>
     <t>Funcional</t>
+  </si>
+  <si>
+    <t>Banco de Dados</t>
+  </si>
+  <si>
+    <t>Aplicação</t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,13 +155,26 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -182,9 +204,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -193,11 +213,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -514,439 +546,545 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762B3419-BE5B-45F0-ACDC-E0F8E076A4B4}">
   <dimension ref="A3:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="88.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="91.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2" t="s">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+      <c r="H3" s="7"/>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B4" s="4">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="D4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="4">
+        <v>8</v>
+      </c>
+      <c r="G4" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
+      <c r="H4" s="7"/>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
       <c r="D5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2" t="s">
+      <c r="F5" s="4">
+        <v>8</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="2">
+      <c r="H5" s="5"/>
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
+      <c r="C6" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2" t="s">
+      <c r="F6" s="4">
+        <v>21</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2">
+      <c r="H6" s="5"/>
+      <c r="I6" s="6"/>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="4">
+        <v>21</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="2">
+      <c r="H7" s="5"/>
+      <c r="I7" s="6"/>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
+      <c r="C8" s="4" t="s">
+        <v>32</v>
+      </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="2">
+      <c r="F8" s="4">
+        <v>21</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H8" s="5"/>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="4">
         <v>6</v>
       </c>
-      <c r="C9" s="2"/>
+      <c r="C9" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2" t="s">
+      <c r="F9" s="4">
+        <v>3</v>
+      </c>
+      <c r="G9" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="2">
+      <c r="H9" s="7"/>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="4">
         <v>7</v>
       </c>
-      <c r="C10" s="2"/>
+      <c r="C10" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="2">
+      <c r="F10" s="4">
+        <v>3</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
         <v>8</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="E11" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="2">
+      <c r="F11" s="4">
+        <v>5</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H11" s="7"/>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="4">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
+      <c r="C12" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="2">
+      <c r="F12" s="4">
+        <v>5</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="4">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
+      <c r="C13" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="2">
+      <c r="F13" s="4">
+        <v>13</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H13" s="5"/>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="4">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
+      <c r="C14" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="2">
+      <c r="F14" s="4">
+        <v>8</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="4">
         <v>12</v>
       </c>
-      <c r="C15" s="2"/>
+      <c r="C15" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="2">
+      <c r="F15" s="4">
         <v>13</v>
       </c>
-      <c r="C16" s="2"/>
+      <c r="G15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="7"/>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="4">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F16" s="4">
+        <v>8</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="2">
+      <c r="B17" s="4">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
+      <c r="C17" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D17" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="E17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F17" s="4">
+        <v>13</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H17" s="7"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="2">
+      <c r="B18" s="4">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
+      <c r="C18" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D18" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F18" s="4">
+        <v>5</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="2">
+      <c r="B19" s="4">
         <v>16</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F19" s="4">
+        <v>8</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" s="7"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="2">
+      <c r="B20" s="4">
         <v>17</v>
       </c>
-      <c r="C20" s="2"/>
+      <c r="C20" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F20" s="4">
+        <v>8</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="2">
+      <c r="B21" s="4">
         <v>18</v>
       </c>
-      <c r="C21" s="2"/>
+      <c r="C21" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F21" s="4">
+        <v>13</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H21" s="7"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="2">
+      <c r="B22" s="4">
         <v>19</v>
       </c>
-      <c r="C22" s="2"/>
+      <c r="C22" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="G22" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" s="3"/>
+      <c r="F22" s="4">
+        <v>13</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="2">
+      <c r="B23" s="4">
         <v>20</v>
       </c>
-      <c r="C23" s="2"/>
+      <c r="C23" s="4" t="s">
+        <v>33</v>
+      </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="F23" s="4">
+        <v>8</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="H23" s="7"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
-      <c r="E33" s="2"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="2"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>

</xml_diff>